<commit_message>
correcting case for rev 0
</commit_message>
<xml_diff>
--- a/production_BOM/bom_r3_cust.xlsx
+++ b/production_BOM/bom_r3_cust.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-repos\cad-libraries\production_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F6C016-422A-4EBD-AE0E-3E03AB440A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB145087-E83F-4FBC-BC52-C2D2E98920F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>#</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>test_rev_A2</t>
   </si>
 </sst>
 </file>
@@ -573,7 +576,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -617,9 +620,12 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
       <c r="C2" t="str">
-        <f>RIGHT(B2,IF(RIGHT(B2,1)="0",1,2))</f>
-        <v/>
+        <f>RIGHT(B2,IF(RIGHT(B2,1)="0",0,2))</f>
+        <v>A2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing relation for rev 0
</commit_message>
<xml_diff>
--- a/production_BOM/bom_r3_cust.xlsx
+++ b/production_BOM/bom_r3_cust.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-repos\cad-libraries\production_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB145087-E83F-4FBC-BC52-C2D2E98920F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8553EC-2DF5-48E5-ADE9-523DA6FBA409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="2910" windowWidth="28800" windowHeight="15210" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="components request" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>#</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>test_rev_0</t>
   </si>
   <si>
     <t>test_rev_A2</t>
@@ -573,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -624,7 +627,16 @@
         <v>21</v>
       </c>
       <c r="C2" t="str">
-        <f>RIGHT(B2,IF(RIGHT(B2,1)="0",0,2))</f>
+        <f>RIGHT(B2,IF(RIGHT(B2,1)="0",,2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="str">
+        <f>RIGHT(B3,IF(RIGHT(B3,1)="0",,2))</f>
         <v>A2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reverting rule for rev 0 for compatibility with the MWS software
</commit_message>
<xml_diff>
--- a/production_BOM/bom_r3_cust.xlsx
+++ b/production_BOM/bom_r3_cust.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-repos\cad-libraries\production_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8553EC-2DF5-48E5-ADE9-523DA6FBA409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318F6180-D5C6-4B29-83D1-21084776CB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="2910" windowWidth="28800" windowHeight="15210" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24000" yWindow="0" windowWidth="24195" windowHeight="14280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="components request" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -627,8 +627,8 @@
         <v>21</v>
       </c>
       <c r="C2" t="str">
-        <f>RIGHT(B2,IF(RIGHT(B2,1)="0",,2))</f>
-        <v/>
+        <f>RIGHT(B2,IF(RIGHT(B2,1)="0",1,2))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>22</v>
       </c>
       <c r="C3" t="str">
-        <f>RIGHT(B3,IF(RIGHT(B3,1)="0",,2))</f>
+        <f>RIGHT(B3,IF(RIGHT(B3,1)="0",1,2))</f>
         <v>A2</v>
       </c>
     </row>

</xml_diff>